<commit_message>
docs: Demo - Expenses Updated
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560"/>
+    <workbookView windowHeight="21560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="103">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -386,16 +386,15 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>HSBC</t>
+    <t>Mother borrowed $570 For Buying Cigarette Buds</t>
   </si>
   <si>
-    <t>Previous Amount Brought Forward</t>
+    <t>- See the Doctor ~ $125
+- Buy Cigarette Buds ~ $800</t>
   </si>
   <si>
-    <t>- See the Doctor ~ $125</t>
-  </si>
-  <si>
-    <t>- Fuck a prostitute who looks like Bill gates's wife.</t>
+    <t>-Visit prostitute $390
+-Return Trip To Mong Kok ~ $6</t>
   </si>
   <si>
     <t>Balance Brought Forward From July 2024</t>
@@ -2901,7 +2900,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -4698,7 +4697,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -4714,7 +4713,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -4730,7 +4729,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -4746,7 +4745,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -6233,7 +6232,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -6429,7 +6428,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -6445,7 +6444,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -6539,7 +6538,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -6807,7 +6806,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -6899,7 +6898,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -7167,7 +7166,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -7259,7 +7258,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -7527,7 +7526,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -8057,7 +8056,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -8073,7 +8072,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8089,7 +8088,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -8105,7 +8104,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -9592,7 +9591,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -9788,7 +9787,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -9804,7 +9803,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -9898,7 +9897,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -10166,7 +10165,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -10258,7 +10257,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -10526,7 +10525,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -10618,7 +10617,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -10886,7 +10885,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -11417,7 +11416,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -11433,7 +11432,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -11449,7 +11448,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -11465,7 +11464,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -12952,7 +12951,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -13148,7 +13147,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -13164,7 +13163,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -13258,7 +13257,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -13526,7 +13525,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -13618,7 +13617,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -13886,7 +13885,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -13978,7 +13977,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -14246,7 +14245,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -14775,7 +14774,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -14791,7 +14790,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -14807,7 +14806,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14823,7 +14822,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -16310,7 +16309,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -16506,7 +16505,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -16522,7 +16521,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -16616,7 +16615,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -16884,7 +16883,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -16976,7 +16975,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17244,7 +17243,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -17336,7 +17335,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -17604,7 +17603,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18135,7 +18134,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18151,7 +18150,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18167,7 +18166,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -18183,7 +18182,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -19670,7 +19669,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -19866,7 +19865,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -19882,7 +19881,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -19976,7 +19975,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20244,7 +20243,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20336,7 +20335,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -20604,7 +20603,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -20696,7 +20695,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -20964,7 +20963,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -21493,7 +21492,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -21509,7 +21508,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -21525,7 +21524,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21541,7 +21540,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -23028,7 +23027,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -23224,7 +23223,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -23240,7 +23239,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -23334,7 +23333,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23602,7 +23601,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -23694,7 +23693,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -23962,7 +23961,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24054,7 +24053,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24322,7 +24321,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -24852,7 +24851,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -24868,7 +24867,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -24884,7 +24883,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -24900,7 +24899,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -26387,7 +26386,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -26583,7 +26582,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -26599,7 +26598,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -26693,7 +26692,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -26961,7 +26960,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27053,7 +27052,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27321,7 +27320,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27413,7 +27412,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27681,7 +27680,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28158,7 +28157,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28174,7 +28173,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28190,7 +28189,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28206,7 +28205,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -29693,7 +29692,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -29768,7 +29767,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C102" s="36" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -29888,7 +29887,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -29904,7 +29903,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -29998,7 +29997,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -30266,7 +30265,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30358,7 +30357,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30626,7 +30625,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -30718,7 +30717,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -30986,7 +30985,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31465,7 +31464,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31481,7 +31480,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31497,7 +31496,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31513,7 +31512,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -33000,7 +32999,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="68"/>
@@ -33196,7 +33195,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -33212,7 +33211,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -33306,7 +33305,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -33574,7 +33573,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -33666,7 +33665,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -33934,7 +33933,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -34026,7 +34025,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -34294,7 +34293,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -34732,7 +34731,7 @@
   <sheetPr/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B51" sqref="B51:B53"/>
     </sheetView>
   </sheetViews>
@@ -35276,8 +35275,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -35347,7 +35346,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="163">
-        <v>94.4</v>
+        <v>99.4</v>
       </c>
       <c r="D3" s="164" t="s">
         <v>34</v>
@@ -35356,7 +35355,7 @@
         <v>35</v>
       </c>
       <c r="F3" s="190">
-        <v>0</v>
+        <v>594.4</v>
       </c>
       <c r="I3" s="198" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -35364,7 +35363,7 @@
       </c>
       <c r="J3" s="199">
         <f>E149</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
       <c r="M3" s="204" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,3)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+2),"dd mmmm yyyy"))</f>
@@ -35372,7 +35371,7 @@
       </c>
       <c r="N3" s="199">
         <f>-C122</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="4" ht="35.25" customHeight="1" spans="1:14">
@@ -35381,14 +35380,14 @@
         <v>36</v>
       </c>
       <c r="C4" s="163">
-        <v>270</v>
+        <v>840</v>
       </c>
       <c r="D4" s="165"/>
       <c r="E4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="190">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="I4" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
@@ -35396,7 +35395,7 @@
       </c>
       <c r="J4" s="199">
         <f>E176</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
       <c r="M4" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,3),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+3),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,6)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*6+5),"dd mmmm yyyy"))</f>
@@ -35404,7 +35403,7 @@
       </c>
       <c r="N4" s="199">
         <f ca="1">'April 2025 - June 2025'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="5" ht="35.25" customHeight="1" spans="1:14">
@@ -35428,7 +35427,7 @@
       </c>
       <c r="J5" s="199">
         <f>E203</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
       <c r="M5" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,6),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*6+6),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,9)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*9+8),"dd mmmm yyyy"))</f>
@@ -35436,7 +35435,7 @@
       </c>
       <c r="N5" s="199">
         <f ca="1">'July 2025 - September 2025'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="6" ht="35.25" customHeight="1" spans="1:14">
@@ -35460,7 +35459,7 @@
       </c>
       <c r="J6" s="199">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="M6" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,9),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*9+9),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,12)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+11),"dd mmmm yyyy"))</f>
@@ -35468,7 +35467,7 @@
       </c>
       <c r="N6" s="199">
         <f ca="1">'October 2025 - December 2025'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="7" ht="35.25" customHeight="1" spans="1:14">
@@ -35477,14 +35476,14 @@
         <v>39</v>
       </c>
       <c r="C7" s="163">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7" s="165"/>
       <c r="E7" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="190">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I7" s="201" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,4),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*4)+4,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,5)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*5+4),"dd mmmm yyyy"))</f>
@@ -35492,7 +35491,7 @@
       </c>
       <c r="J7" s="199">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>2580.71</v>
+        <v>3150.71</v>
       </c>
       <c r="M7" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,12),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+12),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,15)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+14),"dd mmmm yyyy"))</f>
@@ -35500,7 +35499,7 @@
       </c>
       <c r="N7" s="199">
         <f ca="1">'January 2026 - March 2026'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="8" ht="45" customHeight="1" spans="1:14">
@@ -35525,7 +35524,7 @@
       </c>
       <c r="J8" s="199">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>4615.71</v>
+        <v>5185.71</v>
       </c>
       <c r="M8" s="207" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+15),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
@@ -35533,7 +35532,7 @@
       </c>
       <c r="N8" s="199">
         <f ca="1">'April 2026 - June 2026'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="9" ht="39.75" customHeight="1" spans="1:14">
@@ -35557,7 +35556,7 @@
       </c>
       <c r="J9" s="199">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>6650.71</v>
+        <v>7220.71</v>
       </c>
       <c r="M9" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+18),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,21)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+20),"dd mmmm yyyy"))</f>
@@ -35565,7 +35564,7 @@
       </c>
       <c r="N9" s="208">
         <f ca="1">'July 2026 - September 2026'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="10" ht="35.25" customHeight="1" spans="1:14">
@@ -35589,7 +35588,7 @@
       </c>
       <c r="J10" s="199">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>8685.71</v>
+        <v>9255.71</v>
       </c>
       <c r="M10" s="209" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
@@ -35597,7 +35596,7 @@
       </c>
       <c r="N10" s="199">
         <f ca="1">'October 2026 - December 2026'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="11" ht="35.25" customHeight="1" spans="1:14">
@@ -35613,7 +35612,7 @@
         <v>43</v>
       </c>
       <c r="F11" s="190">
-        <v>0</v>
+        <v>29.4</v>
       </c>
       <c r="H11" s="191"/>
       <c r="I11" s="200" t="str">
@@ -35622,7 +35621,7 @@
       </c>
       <c r="J11" s="199">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>10720.71</v>
+        <v>11290.71</v>
       </c>
       <c r="M11" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,24),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+24),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,27)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+26),"dd mmmm yyyy"))</f>
@@ -35630,7 +35629,7 @@
       </c>
       <c r="N11" s="203">
         <f ca="1">'January 2027 - March 2027'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" spans="1:14">
@@ -35646,7 +35645,7 @@
         <v>44</v>
       </c>
       <c r="F12" s="190">
-        <v>0</v>
+        <v>118.01</v>
       </c>
       <c r="I12" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,9),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*9)+9,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,10)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*10+9),"dd mmmm yyyy"))</f>
@@ -35654,7 +35653,7 @@
       </c>
       <c r="J12" s="199">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>12755.71</v>
+        <v>13325.71</v>
       </c>
       <c r="M12" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27+27),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
@@ -35662,7 +35661,7 @@
       </c>
       <c r="N12" s="203">
         <f ca="1">'April 2027 - June 2027'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="13" ht="35.25" customHeight="1" spans="1:14">
@@ -35678,7 +35677,7 @@
         <v>45</v>
       </c>
       <c r="F13" s="190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,10),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*10)+10,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,11)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*11+10),"dd mmmm yyyy"))</f>
@@ -35686,7 +35685,7 @@
       </c>
       <c r="J13" s="199">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>14790.71</v>
+        <v>15360.71</v>
       </c>
       <c r="M13" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -35694,7 +35693,7 @@
       </c>
       <c r="N13" s="203">
         <f ca="1">'July 2027 - September 2027'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="14" ht="35.25" customHeight="1" spans="1:14">
@@ -35710,7 +35709,7 @@
         <v>46</v>
       </c>
       <c r="F14" s="190">
-        <v>0</v>
+        <v>23.9</v>
       </c>
       <c r="I14" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,11),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*11)+11,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,12)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+11),"dd mmmm yyyy"))</f>
@@ -35718,7 +35717,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>16825.71</v>
+        <v>17395.71</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -35726,7 +35725,7 @@
       </c>
       <c r="N14" s="203">
         <f ca="1">'October 2027 - December 2027'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="15" ht="35.25" customHeight="1" spans="1:14">
@@ -35750,7 +35749,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>18860.71</v>
+        <v>19430.71</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -35758,7 +35757,7 @@
       </c>
       <c r="N15" s="203">
         <f ca="1">'January 2028 - March 2028'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="16" ht="35.25" customHeight="1" spans="1:14">
@@ -35768,7 +35767,7 @@
       </c>
       <c r="C16" s="169">
         <f>SUM(C3:C15)</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D16" s="170"/>
       <c r="E16" s="168" t="s">
@@ -35776,7 +35775,7 @@
       </c>
       <c r="F16" s="193">
         <f>SUM(F3:F15)</f>
-        <v>0</v>
+        <v>941.71</v>
       </c>
       <c r="I16" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -35784,7 +35783,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>20895.71</v>
+        <v>21465.71</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -35792,7 +35791,7 @@
       </c>
       <c r="N16" s="203">
         <f ca="1">'April 2028 - June 2028'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="17" ht="35.25" customHeight="1" spans="9:14">
@@ -35802,7 +35801,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>22930.71</v>
+        <v>23500.71</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -35810,7 +35809,7 @@
       </c>
       <c r="N17" s="203">
         <f ca="1">'July 2028 - September 2028'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="18" ht="35.25" customHeight="1" spans="9:14">
@@ -35820,7 +35819,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>24965.71</v>
+        <v>25535.71</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -35828,7 +35827,7 @@
       </c>
       <c r="N18" s="199">
         <f ca="1">'October 2028 - December 2028'!C5</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
     </row>
     <row r="19" ht="33" customHeight="1" spans="9:10">
@@ -35838,7 +35837,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>27000.71</v>
+        <v>27570.71</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -35848,7 +35847,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>29035.71</v>
+        <v>29605.71</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -35858,7 +35857,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>31070.71</v>
+        <v>31640.71</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -35878,7 +35877,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>33105.71</v>
+        <v>33675.71</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -35903,7 +35902,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="24" ht="33" customHeight="1" spans="1:10">
@@ -35922,7 +35921,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -35941,7 +35940,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -35960,7 +35959,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -35979,7 +35978,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -35998,7 +35997,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -36017,7 +36016,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -36039,7 +36038,7 @@
       </c>
       <c r="J30" s="205">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -36049,7 +36048,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -36059,7 +36058,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -36069,7 +36068,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'July 2027 - September 2027'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -36089,7 +36088,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'July 2027 - September 2027'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -36114,7 +36113,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'July 2027 - September 2027'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1" spans="1:10">
@@ -36137,7 +36136,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'October 2027 - December 2027'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -36156,7 +36155,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'October 2027 - December 2027'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -36175,7 +36174,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'October 2027 - December 2027'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -36194,7 +36193,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'January 2028 - March 2028'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -36213,7 +36212,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'January 2028 - March 2028'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -36232,7 +36231,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'January 2028 - March 2028'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -36254,7 +36253,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">'April 2028 - June 2028'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -36264,7 +36263,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">'April 2028 - June 2028'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -36274,7 +36273,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">'April 2028 - June 2028'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -36284,7 +36283,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">'July 2028 - September 2028'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -36304,7 +36303,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">'July 2028 - September 2028'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -36329,7 +36328,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">'July 2028 - September 2028'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -36352,7 +36351,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">'October 2028 - December 2028'!E136</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -36371,7 +36370,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">'October 2028 - December 2028'!E163</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -36390,7 +36389,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">'October 2028 - December 2028'!E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
     </row>
     <row r="51" ht="41.1" customHeight="1" spans="1:7">
@@ -36880,7 +36879,7 @@
       </c>
       <c r="B112" s="218"/>
       <c r="C112" s="219">
-        <v>5400</v>
+        <v>5970</v>
       </c>
       <c r="D112" s="14"/>
       <c r="E112" s="94"/>
@@ -37013,7 +37012,7 @@
       </c>
       <c r="C122" s="210">
         <f>SUM(C112:C121)</f>
-        <v>6483</v>
+        <v>7053</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -37023,7 +37022,7 @@
       </c>
       <c r="C123" s="36">
         <f>C122+C110</f>
-        <v>6883</v>
+        <v>7453</v>
       </c>
     </row>
     <row r="124" spans="5:5">
@@ -37270,7 +37269,7 @@
       </c>
       <c r="D149" s="81"/>
       <c r="E149" s="87">
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
     </row>
     <row r="150" ht="21.75" customHeight="1"/>
@@ -37307,7 +37306,7 @@
       <c r="D156" s="224"/>
       <c r="E156" s="87">
         <f>E149</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
     </row>
     <row r="157" ht="24.75" customHeight="1" spans="1:5">
@@ -37525,7 +37524,7 @@
       <c r="D176" s="81"/>
       <c r="E176" s="90">
         <f>(F42+E156)-(SUM(E159:E167)+SUM(E169:E175))</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
     </row>
     <row r="180" ht="24.75" customHeight="1"/>
@@ -37562,7 +37561,7 @@
       <c r="D183" s="224"/>
       <c r="E183" s="90">
         <f>E176</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
     </row>
     <row r="184" ht="24.75" customHeight="1" spans="1:5">
@@ -37780,7 +37779,7 @@
       <c r="D203" s="81"/>
       <c r="E203" s="90">
         <f>(F54+E183)-(SUM(E185:E194)+SUM(E196:E202))</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
     </row>
     <row r="204" ht="24.75" customHeight="1"/>
@@ -38248,8 +38247,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E12"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -38286,7 +38285,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -38300,7 +38299,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4615.71</v>
+        <v>5185.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -38314,7 +38313,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5161.42</v>
+        <v>6301.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -38330,7 +38329,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -38431,15 +38430,15 @@
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="135"/>
       <c r="B12" s="113" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C12" s="114"/>
       <c r="D12" s="126" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="146"/>
       <c r="F12" s="41">
-        <v>390</v>
+        <v>570</v>
       </c>
       <c r="G12" s="42"/>
       <c r="H12" s="14"/>
@@ -38494,7 +38493,7 @@
       <c r="E16" s="44"/>
       <c r="F16" s="45">
         <f>SUM(F10:G15)</f>
-        <v>790</v>
+        <v>970</v>
       </c>
       <c r="G16" s="46"/>
       <c r="H16" s="14"/>
@@ -39841,7 +39840,7 @@
       </c>
       <c r="C98" s="108" cm="1">
         <f ca="1" t="array" ref="C98">(((INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E131")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E158")+INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E185")))+SUM(E118+E145+E172))-INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!C112")</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -40036,7 +40035,7 @@
       </c>
       <c r="C108" s="108">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -40052,7 +40051,7 @@
       </c>
       <c r="C109" s="108">
         <f ca="1">C108-C96</f>
-        <v>-6883</v>
+        <v>-7453</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -40146,7 +40145,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="87" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B9")&amp;"'!E203")</f>
-        <v>545.71</v>
+        <v>941.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -40314,8 +40313,8 @@
     <row r="129" ht="40.5" customHeight="1" spans="1:9">
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
-      <c r="C129" s="109" t="s">
-        <v>99</v>
+      <c r="C129" s="100" t="s">
+        <v>98</v>
       </c>
       <c r="D129" s="109"/>
       <c r="E129" s="98">
@@ -40326,15 +40325,15 @@
       <c r="H129" s="14"/>
       <c r="I129" s="47"/>
     </row>
-    <row r="130" ht="29" customHeight="1" spans="1:9">
+    <row r="130" ht="47" customHeight="1" spans="1:9">
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D130" s="109"/>
       <c r="E130" s="98">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -40418,7 +40417,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -40510,7 +40509,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -40778,7 +40777,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>2580.71</v>
+        <v>3150.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -40862,14 +40861,14 @@
     </row>
     <row r="170" ht="24.75" customHeight="1" spans="1:9">
       <c r="A170" s="55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B170" s="56"/>
       <c r="C170" s="57"/>
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>2580.71</v>
+        <v>3150.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -41137,7 +41136,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4615.71</v>
+        <v>5185.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -41618,7 +41617,7 @@
   <sheetPr/>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
+    <sheetView topLeftCell="A111" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
@@ -41652,7 +41651,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -41666,7 +41665,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10720.71</v>
+        <v>11290.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -41680,7 +41679,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11266.42</v>
+        <v>12406.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -41696,7 +41695,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -43195,7 +43194,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -43391,7 +43390,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -43407,7 +43406,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6883</v>
+        <v>-7453</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -43501,7 +43500,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="87" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B12")&amp;"'!E190")</f>
-        <v>4615.71</v>
+        <v>5185.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -43769,7 +43768,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>6650.71</v>
+        <v>7220.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -43861,7 +43860,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>6650.71</v>
+        <v>7220.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -44129,7 +44128,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>8685.71</v>
+        <v>9255.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -44221,7 +44220,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>8685.71</v>
+        <v>9255.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -44489,7 +44488,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10720.71</v>
+        <v>11290.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -45074,7 +45073,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -45090,7 +45089,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>16825.71</v>
+        <v>17395.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -45106,7 +45105,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>17371.42</v>
+        <v>18511.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -45122,7 +45121,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -46621,7 +46620,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -46817,7 +46816,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -46833,7 +46832,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6883</v>
+        <v>-7453</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -46927,7 +46926,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B15")&amp;"'!E190")</f>
-        <v>10720.71</v>
+        <v>11290.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -47195,7 +47194,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12755.71</v>
+        <v>13325.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -47287,7 +47286,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12755.71</v>
+        <v>13325.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -47555,7 +47554,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14790.71</v>
+        <v>15360.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -47647,7 +47646,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>14790.71</v>
+        <v>15360.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -47915,7 +47914,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16825.71</v>
+        <v>17395.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -48490,7 +48489,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48506,7 +48505,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>22930.71</v>
+        <v>23500.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -48522,7 +48521,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>23476.42</v>
+        <v>24616.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -48538,7 +48537,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -50037,7 +50036,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -50233,7 +50232,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -50249,7 +50248,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-6883</v>
+        <v>-7453</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -50343,7 +50342,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>16825.71</v>
+        <v>17395.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -50611,7 +50610,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>18860.71</v>
+        <v>19430.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -50703,7 +50702,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>18860.71</v>
+        <v>19430.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -50971,7 +50970,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>20895.71</v>
+        <v>21465.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -51063,7 +51062,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>20895.71</v>
+        <v>21465.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -51331,7 +51330,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>22930.71</v>
+        <v>23500.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -51872,7 +51871,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -51888,7 +51887,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>29035.71</v>
+        <v>29605.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -51904,7 +51903,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>29581.42</v>
+        <v>30721.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -51920,7 +51919,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -53419,7 +53418,7 @@
       </c>
       <c r="C98" s="108" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -53615,7 +53614,7 @@
       </c>
       <c r="C108" s="108">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -53631,7 +53630,7 @@
       </c>
       <c r="C109" s="108">
         <f ca="1">C108-C96</f>
-        <v>-6883</v>
+        <v>-7453</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -53725,7 +53724,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>22930.71</v>
+        <v>23500.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -53993,7 +53992,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>24965.71</v>
+        <v>25535.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -54085,7 +54084,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>24965.71</v>
+        <v>25535.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -54353,7 +54352,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>27000.71</v>
+        <v>27570.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -54445,7 +54444,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>27000.71</v>
+        <v>27570.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -54713,7 +54712,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>29035.71</v>
+        <v>29605.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -55257,7 +55256,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>545.71</v>
+        <v>1115.71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -55273,7 +55272,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -55289,7 +55288,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35686.42</v>
+        <v>36826.42</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55305,7 +55304,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -55388,7 +55387,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="96"/>
       <c r="C11" s="96"/>
@@ -56806,7 +56805,7 @@
       </c>
       <c r="C98" s="108" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5400</v>
+        <v>-5970</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -57002,7 +57001,7 @@
       </c>
       <c r="C108" s="108">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6483</v>
+        <v>-7053</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -57018,7 +57017,7 @@
       </c>
       <c r="C109" s="108">
         <f ca="1">C108-C96</f>
-        <v>-6883</v>
+        <v>-7453</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -57112,7 +57111,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>29035.71</v>
+        <v>29605.71</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -57380,7 +57379,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>31070.71</v>
+        <v>31640.71</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -57472,7 +57471,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>31070.71</v>
+        <v>31640.71</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -57740,7 +57739,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>33105.71</v>
+        <v>33675.71</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -57832,7 +57831,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>33105.71</v>
+        <v>33675.71</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -58100,7 +58099,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35140.71</v>
+        <v>35710.71</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>